<commit_message>
Update data processing and analysis code --> blood gas only sensitivity
</commit_message>
<xml_diff>
--- a/results/2_logreg/LogisticRegressionGlucoseDayOne.xlsx
+++ b/results/2_logreg/LogisticRegressionGlucoseDayOne.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.383139112850852</v>
+        <v>0.9488411582465469</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5513833998028874</v>
+        <v>0.407354605155226</v>
       </c>
       <c r="E2" t="n">
-        <v>3.469589048530914</v>
+        <v>2.210112595240163</v>
       </c>
     </row>
     <row r="3">
@@ -488,13 +488,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.71537560989207</v>
+        <v>1.253413971888949</v>
       </c>
       <c r="D3" t="n">
-        <v>1.433981241416687</v>
+        <v>1.107642987878564</v>
       </c>
       <c r="E3" t="n">
-        <v>2.051988825255179</v>
+        <v>1.418369097370815</v>
       </c>
     </row>
     <row r="4">
@@ -509,13 +509,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.001330086320363</v>
+        <v>0.9723939511214528</v>
       </c>
       <c r="D4" t="n">
-        <v>0.838141043314107</v>
+        <v>0.8381951595210121</v>
       </c>
       <c r="E4" t="n">
-        <v>1.196292616581218</v>
+        <v>1.128078569098307</v>
       </c>
     </row>
     <row r="5">
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.04965162906585</v>
+        <v>0.9903870926872311</v>
       </c>
       <c r="D5" t="n">
-        <v>1.028714718582503</v>
+        <v>0.9733128763468433</v>
       </c>
       <c r="E5" t="n">
-        <v>1.071014657901224</v>
+        <v>1.007760831278606</v>
       </c>
     </row>
     <row r="6">
@@ -551,13 +551,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.087408937031029</v>
+        <v>1.197627154790709</v>
       </c>
       <c r="D6" t="n">
-        <v>1.071301527139887</v>
+        <v>1.184477668066314</v>
       </c>
       <c r="E6" t="n">
-        <v>1.103758527715186</v>
+        <v>1.210922620629592</v>
       </c>
     </row>
     <row r="7">
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9953458831978578</v>
+        <v>0.9973503141322366</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9915964259091715</v>
+        <v>0.9939883257945266</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9991095180587823</v>
+        <v>1.000723673796239</v>
       </c>
     </row>
     <row r="8">
@@ -593,13 +593,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.088810093646597</v>
+        <v>0.9917223146622363</v>
       </c>
       <c r="D8" t="n">
-        <v>0.90472993348624</v>
+        <v>0.8557189263274573</v>
       </c>
       <c r="E8" t="n">
-        <v>1.310343977963168</v>
+        <v>1.149341353965406</v>
       </c>
     </row>
     <row r="9">
@@ -614,13 +614,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.924388693394439</v>
+        <v>6.57006563924765</v>
       </c>
       <c r="D9" t="n">
-        <v>1.733017410895656</v>
+        <v>6.027333300987554</v>
       </c>
       <c r="E9" t="n">
-        <v>2.136892462811689</v>
+        <v>7.161668410962123</v>
       </c>
     </row>
     <row r="10">
@@ -635,13 +635,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9787730272151537</v>
+        <v>1.022393387768628</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8222506588450894</v>
+        <v>0.8750852033297862</v>
       </c>
       <c r="E10" t="n">
-        <v>1.165090752434898</v>
+        <v>1.194498816087377</v>
       </c>
     </row>
     <row r="11">
@@ -656,13 +656,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8249822069369648</v>
+        <v>1.069636368392201</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6522978514633623</v>
+        <v>0.91823621251535</v>
       </c>
       <c r="E11" t="n">
-        <v>1.043381700914298</v>
+        <v>1.245999607718727</v>
       </c>
     </row>
     <row r="12">
@@ -677,13 +677,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9366266613390759</v>
+        <v>0.9852563497576496</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8551585005560487</v>
+        <v>0.9105167048164537</v>
       </c>
       <c r="E12" t="n">
-        <v>1.025856028047149</v>
+        <v>1.066130988704323</v>
       </c>
     </row>
     <row r="13">
@@ -698,13 +698,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9758932233655427</v>
+        <v>0.898572494923975</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8354064376962427</v>
+        <v>0.7906746335718713</v>
       </c>
       <c r="E13" t="n">
-        <v>1.140005080685138</v>
+        <v>1.021194426064135</v>
       </c>
     </row>
     <row r="14">
@@ -719,13 +719,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.054994804427525</v>
+        <v>0.8838844303016808</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9306050789880532</v>
+        <v>0.796355427133532</v>
       </c>
       <c r="E14" t="n">
-        <v>1.196011135657427</v>
+        <v>0.9810339196680422</v>
       </c>
     </row>
     <row r="15">
@@ -740,13 +740,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9039583771637588</v>
+        <v>0.9469882888737423</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8096008785513744</v>
+        <v>0.8585160232803121</v>
       </c>
       <c r="E15" t="n">
-        <v>1.009313069307253</v>
+        <v>1.044577847059251</v>
       </c>
     </row>
     <row r="16">
@@ -761,13 +761,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.050350098762067</v>
+        <v>1.041734379825617</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8180224246878588</v>
+        <v>0.8426191018382777</v>
       </c>
       <c r="E16" t="n">
-        <v>1.348661475130656</v>
+        <v>1.287901634016061</v>
       </c>
     </row>
     <row r="17">
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1.004176224324602</v>
+        <v>0.9343034340384859</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8706387662772626</v>
+        <v>0.8201330176576371</v>
       </c>
       <c r="E17" t="n">
-        <v>1.158195486528208</v>
+        <v>1.064367472180601</v>
       </c>
     </row>
     <row r="18">
@@ -803,13 +803,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.8006490791743716</v>
+        <v>0.9034324262804929</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6234984281247334</v>
+        <v>0.7133777418229791</v>
       </c>
       <c r="E18" t="n">
-        <v>1.028132420334709</v>
+        <v>1.144120570357789</v>
       </c>
     </row>
     <row r="19">
@@ -824,13 +824,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.9654392770257932</v>
+        <v>1.03448441586587</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8713932371044801</v>
+        <v>0.9483984944080451</v>
       </c>
       <c r="E19" t="n">
-        <v>1.069635335616371</v>
+        <v>1.128384337363697</v>
       </c>
     </row>
     <row r="20">
@@ -845,13 +845,30 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.8620833863301826</v>
+        <v>0.9810424703866519</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7217399954024105</v>
+        <v>0.8335894966537385</v>
       </c>
       <c r="E20" t="n">
-        <v>1.029716753568778</v>
+        <v>1.15457828171524</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>const</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>0.02458040599925118</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.01844754074416798</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.03275213577067364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>